<commit_message>
local changes to the file
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>@4:10 Am</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>reach room</t>
+          <t>fdhxfgh</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>no ditraction</t>
+          <t>vcgh</t>
         </is>
       </c>
     </row>
@@ -481,17 +481,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>@4:30 AM</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>start studying</t>
+          <t>xfgh</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>dfsdf</t>
+          <t>fgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>fgjn</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>fgjn</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to save new file locally
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,46 +455,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>@4:10 Am</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>reach room</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>no ditraction</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>@4:30 AM</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>start studying</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>dfsdf</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>